<commit_message>
Resultados de WebSraping y procesamiento de Caracol Gigante
</commit_message>
<xml_diff>
--- a/BDCARACOL.xlsx
+++ b/BDCARACOL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57314\Documents\LEONARDO\CAR\CAR 2022\CONTRATO 2 - 2473\INFORMES VTIC\3. CARACOL AFRICANO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57314\Documents\LEONARDO\CAR\CODIGOS\WebScraping MinCiencias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423FB21B-433E-4B34-9561-6387773FF669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BD93B5-1DEE-431E-99DD-2457D113B6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t xml:space="preserve">NOMBRE </t>
   </si>
   <si>
-    <t xml:space="preserve">LINKS </t>
-  </si>
-  <si>
     <t>Territorios Semiáridos del Caribe</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>Agua y desarrollo sostenible en Ingenierías GRUPO AQUA</t>
+  </si>
+  <si>
+    <t>LINKS</t>
   </si>
 </sst>
 </file>
@@ -316,7 +316,7 @@
   <autoFilter ref="A1:B23" xr:uid="{3ED6AA16-FDBE-4888-9E2A-ACAE671A7331}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{831632AE-2534-4F99-9864-F229EAC92CB1}" name="NOMBRE " dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{D8041A12-BC48-4F50-A5CA-8DE565E6654C}" name="LINKS " dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{D8041A12-BC48-4F50-A5CA-8DE565E6654C}" name="LINKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -588,7 +588,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,183 +602,183 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>